<commit_message>
Ubicacion fija, nivelacion con mas detalle y menos texto, mejora en los 3 sobre totales, mejora en los 3 sobre currency
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -11,7 +11,7 @@
     <sheet name="JDN-Cot-TL-201011" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'JDN-Cot-TL-201011'!$A$1:$E$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'JDN-Cot-TL-201011'!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve">JDN COMPANY RIEGO</t>
   </si>
@@ -55,25 +55,43 @@
     <t xml:space="preserve">Estacado de la laguna</t>
   </si>
   <si>
-    <t xml:space="preserve">Estacado de quebracho  3 Tablas, puntales de quebracho entero, tablas de medio durmiente </t>
-  </si>
-  <si>
-    <t xml:space="preserve">riendas con varillas roscadas de 13mm, geotextil, cuplas, arandelas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mano de obra incluida. 20    mts lineales.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Puntales de 4 pulg x 9 pulg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.40</t>
+    <t xml:space="preserve">Estacado </t>
   </si>
   <si>
     <t xml:space="preserve">Escalones</t>
   </si>
   <si>
     <t xml:space="preserve">Sub Total $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mano de obra incluida mts lineales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estacado de quebracho 3 Tablas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tablas de medio durmiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">riendas con varillas roscadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geotextil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cuplas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arandelas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puntales en pulgadas</t>
   </si>
   <si>
     <t xml:space="preserve">CONDICIÓN DE PAGO</t>
@@ -119,6 +137,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,12 +159,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial Black"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -153,11 +174,13 @@
       <color rgb="FF000090"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -165,6 +188,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -172,17 +196,20 @@
       <color rgb="FF000090"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="20"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -191,12 +218,14 @@
       <color rgb="FFDD0806"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -231,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -323,9 +352,15 @@
       <left style="medium">
         <color rgb="FF3D3D3D"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="medium">
+        <color rgb="FF3D3D3D"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF3D3D3D"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF3D3D3D"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -355,18 +390,54 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FF3D3D3D"/>
       </left>
-      <right style="medium">
-        <color rgb="FF3D3D3D"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF3D3D3D"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF3D3D3D"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -413,11 +484,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,11 +547,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,23 +563,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,7 +591,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,11 +599,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="10" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="12" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="14" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,7 +663,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -566,7 +679,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -574,7 +687,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -582,7 +695,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,18 +771,60 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4879080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9085320</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>427680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7351200" y="5624640"/>
+          <a:ext cx="4206240" cy="2905560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ402"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.8"/>
@@ -1427,7 +1582,7 @@
       <c r="BZ9" s="2"/>
       <c r="CA9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15" t="s">
@@ -1510,20 +1665,16 @@
       <c r="BZ10" s="2"/>
       <c r="CA10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
-      <c r="B11" s="14" t="n">
-        <v>20</v>
-      </c>
+      <c r="B11" s="14"/>
       <c r="C11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="16" t="n">
-        <v>130000</v>
-      </c>
+      <c r="D11" s="16"/>
       <c r="E11" s="17" t="n">
         <f aca="false">B11*D11</f>
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1600,12 +1751,10 @@
       <c r="BZ11" s="2"/>
       <c r="CA11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="C12" s="18"/>
       <c r="D12" s="16"/>
       <c r="E12" s="17"/>
       <c r="F12" s="2"/>
@@ -1683,14 +1832,17 @@
       <c r="BZ12" s="2"/>
       <c r="CA12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="19" t="s">
-        <v>12</v>
+      <c r="C13" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="E13" s="17" t="n">
+        <f aca="false">D13*B13</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1766,12 +1918,10 @@
       <c r="BZ13" s="2"/>
       <c r="CA13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="18" t="s">
-        <v>13</v>
-      </c>
+    <row r="14" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17"/>
       <c r="F14" s="2"/>
@@ -1849,19 +1999,16 @@
       <c r="BZ14" s="2"/>
       <c r="CA14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
-        <v>14</v>
+    <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
+        <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="16" t="n">
-        <v>36000</v>
-      </c>
-      <c r="E15" s="17" t="n">
-        <v>302400</v>
+      <c r="E15" s="24" t="n">
+        <f aca="false">SUM(E11:E14)</f>
+        <v>0</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1938,12 +2085,12 @@
       <c r="BZ15" s="2"/>
       <c r="CA15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2019,12 +2166,14 @@
       <c r="BZ16" s="2"/>
       <c r="CA16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
+    <row r="17" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="29"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -2100,12 +2249,14 @@
       <c r="BZ17" s="2"/>
       <c r="CA17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
+    <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2181,12 +2332,17 @@
       <c r="BZ18" s="2"/>
       <c r="CA18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+    <row r="19" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="34"/>
+      <c r="B19" s="30" t="n">
+        <f aca="false">B11</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2262,12 +2418,16 @@
       <c r="BZ19" s="2"/>
       <c r="CA19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
+    <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34"/>
+      <c r="B20" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2343,17 +2503,16 @@
       <c r="BZ20" s="2"/>
       <c r="CA20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23" t="s">
-        <v>16</v>
+    <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="34"/>
+      <c r="B21" s="30" t="s">
+        <v>15</v>
       </c>
-      <c r="E21" s="24" t="n">
-        <f aca="false">SUM(E11:E20)</f>
-        <v>2902400</v>
+      <c r="C21" s="34" t="s">
+        <v>17</v>
       </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2429,12 +2588,14 @@
       <c r="BZ21" s="2"/>
       <c r="CA21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="26"/>
+    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="34"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2510,14 +2671,16 @@
       <c r="BZ22" s="2"/>
       <c r="CA22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="27" t="s">
-        <v>8</v>
+    <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="34"/>
+      <c r="B23" s="30" t="s">
+        <v>15</v>
       </c>
-      <c r="E23" s="28"/>
+      <c r="C23" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2593,12 +2756,16 @@
       <c r="BZ23" s="2"/>
       <c r="CA23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+    <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="34"/>
+      <c r="B24" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2673,41 +2840,17 @@
       <c r="BY24" s="2"/>
       <c r="BZ24" s="2"/>
       <c r="CA24" s="2"/>
-      <c r="CB24" s="2"/>
-      <c r="CC24" s="2"/>
-      <c r="CD24" s="2"/>
-      <c r="CE24" s="2"/>
-      <c r="CF24" s="2"/>
-      <c r="CG24" s="2"/>
-      <c r="CH24" s="2"/>
-      <c r="CI24" s="2"/>
-      <c r="CJ24" s="2"/>
-      <c r="CK24" s="2"/>
-      <c r="CL24" s="2"/>
-      <c r="CM24" s="2"/>
-      <c r="CN24" s="2"/>
-      <c r="CO24" s="2"/>
-      <c r="CP24" s="2"/>
-      <c r="CQ24" s="2"/>
-      <c r="CR24" s="2"/>
-      <c r="CS24" s="2"/>
-      <c r="CT24" s="2"/>
-      <c r="CU24" s="2"/>
-      <c r="CV24" s="2"/>
-      <c r="CW24" s="2"/>
-      <c r="CX24" s="2"/>
-      <c r="CY24" s="2"/>
-      <c r="CZ24" s="2"/>
-      <c r="DA24" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
-        <v>17</v>
+    </row>
+    <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34"/>
+      <c r="B25" s="30" t="s">
+        <v>15</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="C25" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2782,41 +2925,15 @@
       <c r="BY25" s="2"/>
       <c r="BZ25" s="2"/>
       <c r="CA25" s="2"/>
-      <c r="CB25" s="2"/>
-      <c r="CC25" s="2"/>
-      <c r="CD25" s="2"/>
-      <c r="CE25" s="2"/>
-      <c r="CF25" s="2"/>
-      <c r="CG25" s="2"/>
-      <c r="CH25" s="2"/>
-      <c r="CI25" s="2"/>
-      <c r="CJ25" s="2"/>
-      <c r="CK25" s="2"/>
-      <c r="CL25" s="2"/>
-      <c r="CM25" s="2"/>
-      <c r="CN25" s="2"/>
-      <c r="CO25" s="2"/>
-      <c r="CP25" s="2"/>
-      <c r="CQ25" s="2"/>
-      <c r="CR25" s="2"/>
-      <c r="CS25" s="2"/>
-      <c r="CT25" s="2"/>
-      <c r="CU25" s="2"/>
-      <c r="CV25" s="2"/>
-      <c r="CW25" s="2"/>
-      <c r="CX25" s="2"/>
-      <c r="CY25" s="2"/>
-      <c r="CZ25" s="2"/>
-      <c r="DA25" s="2"/>
-    </row>
-    <row r="26" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
-        <v>18</v>
+    </row>
+    <row r="26" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="34"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="34" t="s">
+        <v>22</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2891,41 +3008,13 @@
       <c r="BY26" s="2"/>
       <c r="BZ26" s="2"/>
       <c r="CA26" s="2"/>
-      <c r="CB26" s="2"/>
-      <c r="CC26" s="2"/>
-      <c r="CD26" s="2"/>
-      <c r="CE26" s="2"/>
-      <c r="CF26" s="2"/>
-      <c r="CG26" s="2"/>
-      <c r="CH26" s="2"/>
-      <c r="CI26" s="2"/>
-      <c r="CJ26" s="2"/>
-      <c r="CK26" s="2"/>
-      <c r="CL26" s="2"/>
-      <c r="CM26" s="2"/>
-      <c r="CN26" s="2"/>
-      <c r="CO26" s="2"/>
-      <c r="CP26" s="2"/>
-      <c r="CQ26" s="2"/>
-      <c r="CR26" s="2"/>
-      <c r="CS26" s="2"/>
-      <c r="CT26" s="2"/>
-      <c r="CU26" s="2"/>
-      <c r="CV26" s="2"/>
-      <c r="CW26" s="2"/>
-      <c r="CX26" s="2"/>
-      <c r="CY26" s="2"/>
-      <c r="CZ26" s="2"/>
-      <c r="DA26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+    </row>
+    <row r="27" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -3028,13 +3117,13 @@
       <c r="DA27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="30" t="s">
-        <v>20</v>
+      <c r="A28" s="40" t="s">
+        <v>23</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3137,13 +3226,13 @@
       <c r="DA28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
-        <v>21</v>
+      <c r="A29" s="41" t="s">
+        <v>24</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -3246,11 +3335,13 @@
       <c r="DA29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
+      <c r="A30" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -3353,13 +3444,13 @@
       <c r="DA30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="s">
-        <v>22</v>
+      <c r="A31" s="40" t="s">
+        <v>26</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -3462,13 +3553,13 @@
       <c r="DA31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
-        <v>23</v>
+      <c r="A32" s="41" t="s">
+        <v>27</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3571,11 +3662,11 @@
       <c r="DA32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -3650,13 +3741,41 @@
       <c r="BY33" s="2"/>
       <c r="BZ33" s="2"/>
       <c r="CA33" s="2"/>
-    </row>
-    <row r="34" customFormat="false" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
+      <c r="CB33" s="2"/>
+      <c r="CC33" s="2"/>
+      <c r="CD33" s="2"/>
+      <c r="CE33" s="2"/>
+      <c r="CF33" s="2"/>
+      <c r="CG33" s="2"/>
+      <c r="CH33" s="2"/>
+      <c r="CI33" s="2"/>
+      <c r="CJ33" s="2"/>
+      <c r="CK33" s="2"/>
+      <c r="CL33" s="2"/>
+      <c r="CM33" s="2"/>
+      <c r="CN33" s="2"/>
+      <c r="CO33" s="2"/>
+      <c r="CP33" s="2"/>
+      <c r="CQ33" s="2"/>
+      <c r="CR33" s="2"/>
+      <c r="CS33" s="2"/>
+      <c r="CT33" s="2"/>
+      <c r="CU33" s="2"/>
+      <c r="CV33" s="2"/>
+      <c r="CW33" s="2"/>
+      <c r="CX33" s="2"/>
+      <c r="CY33" s="2"/>
+      <c r="CZ33" s="2"/>
+      <c r="DA33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -3731,15 +3850,41 @@
       <c r="BY34" s="2"/>
       <c r="BZ34" s="2"/>
       <c r="CA34" s="2"/>
+      <c r="CB34" s="2"/>
+      <c r="CC34" s="2"/>
+      <c r="CD34" s="2"/>
+      <c r="CE34" s="2"/>
+      <c r="CF34" s="2"/>
+      <c r="CG34" s="2"/>
+      <c r="CH34" s="2"/>
+      <c r="CI34" s="2"/>
+      <c r="CJ34" s="2"/>
+      <c r="CK34" s="2"/>
+      <c r="CL34" s="2"/>
+      <c r="CM34" s="2"/>
+      <c r="CN34" s="2"/>
+      <c r="CO34" s="2"/>
+      <c r="CP34" s="2"/>
+      <c r="CQ34" s="2"/>
+      <c r="CR34" s="2"/>
+      <c r="CS34" s="2"/>
+      <c r="CT34" s="2"/>
+      <c r="CU34" s="2"/>
+      <c r="CV34" s="2"/>
+      <c r="CW34" s="2"/>
+      <c r="CX34" s="2"/>
+      <c r="CY34" s="2"/>
+      <c r="CZ34" s="2"/>
+      <c r="DA34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39" t="s">
-        <v>24</v>
+      <c r="A35" s="41" t="s">
+        <v>29</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -3814,15 +3959,39 @@
       <c r="BY35" s="2"/>
       <c r="BZ35" s="2"/>
       <c r="CA35" s="2"/>
+      <c r="CB35" s="2"/>
+      <c r="CC35" s="2"/>
+      <c r="CD35" s="2"/>
+      <c r="CE35" s="2"/>
+      <c r="CF35" s="2"/>
+      <c r="CG35" s="2"/>
+      <c r="CH35" s="2"/>
+      <c r="CI35" s="2"/>
+      <c r="CJ35" s="2"/>
+      <c r="CK35" s="2"/>
+      <c r="CL35" s="2"/>
+      <c r="CM35" s="2"/>
+      <c r="CN35" s="2"/>
+      <c r="CO35" s="2"/>
+      <c r="CP35" s="2"/>
+      <c r="CQ35" s="2"/>
+      <c r="CR35" s="2"/>
+      <c r="CS35" s="2"/>
+      <c r="CT35" s="2"/>
+      <c r="CU35" s="2"/>
+      <c r="CV35" s="2"/>
+      <c r="CW35" s="2"/>
+      <c r="CX35" s="2"/>
+      <c r="CY35" s="2"/>
+      <c r="CZ35" s="2"/>
+      <c r="DA35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="47"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -3898,12 +4067,12 @@
       <c r="BZ36" s="2"/>
       <c r="CA36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+    <row r="37" customFormat="false" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -3979,20 +4148,252 @@
       <c r="BZ37" s="2"/>
       <c r="CA37" s="2"/>
     </row>
-    <row r="38" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH38" s="0"/>
-      <c r="AMI38" s="0"/>
-      <c r="AMJ38" s="0"/>
-    </row>
-    <row r="39" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH39" s="0"/>
-      <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
-    </row>
-    <row r="40" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH40" s="0"/>
-      <c r="AMI40" s="0"/>
-      <c r="AMJ40" s="0"/>
+    <row r="38" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+      <c r="AJ38" s="2"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="2"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="2"/>
+      <c r="AW38" s="2"/>
+      <c r="AX38" s="2"/>
+      <c r="AY38" s="2"/>
+      <c r="AZ38" s="2"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="2"/>
+      <c r="BD38" s="2"/>
+      <c r="BE38" s="2"/>
+      <c r="BF38" s="2"/>
+      <c r="BG38" s="2"/>
+      <c r="BH38" s="2"/>
+      <c r="BI38" s="2"/>
+      <c r="BJ38" s="2"/>
+      <c r="BK38" s="2"/>
+      <c r="BL38" s="2"/>
+      <c r="BM38" s="2"/>
+      <c r="BN38" s="2"/>
+      <c r="BO38" s="2"/>
+      <c r="BP38" s="2"/>
+      <c r="BQ38" s="2"/>
+      <c r="BR38" s="2"/>
+      <c r="BS38" s="2"/>
+      <c r="BT38" s="2"/>
+      <c r="BU38" s="2"/>
+      <c r="BV38" s="2"/>
+      <c r="BW38" s="2"/>
+      <c r="BX38" s="2"/>
+      <c r="BY38" s="2"/>
+      <c r="BZ38" s="2"/>
+      <c r="CA38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="2"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39" s="2"/>
+      <c r="AZ39" s="2"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="2"/>
+      <c r="BD39" s="2"/>
+      <c r="BE39" s="2"/>
+      <c r="BF39" s="2"/>
+      <c r="BG39" s="2"/>
+      <c r="BH39" s="2"/>
+      <c r="BI39" s="2"/>
+      <c r="BJ39" s="2"/>
+      <c r="BK39" s="2"/>
+      <c r="BL39" s="2"/>
+      <c r="BM39" s="2"/>
+      <c r="BN39" s="2"/>
+      <c r="BO39" s="2"/>
+      <c r="BP39" s="2"/>
+      <c r="BQ39" s="2"/>
+      <c r="BR39" s="2"/>
+      <c r="BS39" s="2"/>
+      <c r="BT39" s="2"/>
+      <c r="BU39" s="2"/>
+      <c r="BV39" s="2"/>
+      <c r="BW39" s="2"/>
+      <c r="BX39" s="2"/>
+      <c r="BY39" s="2"/>
+      <c r="BZ39" s="2"/>
+      <c r="CA39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="51"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="2"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="2"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="2"/>
+      <c r="AW40" s="2"/>
+      <c r="AX40" s="2"/>
+      <c r="AY40" s="2"/>
+      <c r="AZ40" s="2"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="2"/>
+      <c r="BD40" s="2"/>
+      <c r="BE40" s="2"/>
+      <c r="BF40" s="2"/>
+      <c r="BG40" s="2"/>
+      <c r="BH40" s="2"/>
+      <c r="BI40" s="2"/>
+      <c r="BJ40" s="2"/>
+      <c r="BK40" s="2"/>
+      <c r="BL40" s="2"/>
+      <c r="BM40" s="2"/>
+      <c r="BN40" s="2"/>
+      <c r="BO40" s="2"/>
+      <c r="BP40" s="2"/>
+      <c r="BQ40" s="2"/>
+      <c r="BR40" s="2"/>
+      <c r="BS40" s="2"/>
+      <c r="BT40" s="2"/>
+      <c r="BU40" s="2"/>
+      <c r="BV40" s="2"/>
+      <c r="BW40" s="2"/>
+      <c r="BX40" s="2"/>
+      <c r="BY40" s="2"/>
+      <c r="BZ40" s="2"/>
+      <c r="CA40" s="2"/>
     </row>
     <row r="41" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AMH41" s="0"/>
@@ -4244,233 +4645,20 @@
       <c r="AMI90" s="0"/>
       <c r="AMJ90" s="0"/>
     </row>
-    <row r="91" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
-      <c r="M91" s="2"/>
-      <c r="N91" s="2"/>
-      <c r="O91" s="2"/>
-      <c r="P91" s="2"/>
-      <c r="Q91" s="2"/>
-      <c r="R91" s="2"/>
-      <c r="S91" s="2"/>
-      <c r="T91" s="2"/>
-      <c r="U91" s="2"/>
-      <c r="V91" s="2"/>
-      <c r="W91" s="2"/>
-      <c r="X91" s="2"/>
-      <c r="Y91" s="2"/>
-      <c r="Z91" s="2"/>
-      <c r="AA91" s="2"/>
-      <c r="AB91" s="2"/>
-      <c r="AC91" s="2"/>
-      <c r="AD91" s="2"/>
-      <c r="AE91" s="2"/>
-      <c r="AF91" s="2"/>
-      <c r="AG91" s="2"/>
-      <c r="AH91" s="2"/>
-      <c r="AI91" s="2"/>
-      <c r="AJ91" s="2"/>
-      <c r="AK91" s="2"/>
-      <c r="AL91" s="2"/>
-      <c r="AM91" s="2"/>
-      <c r="AN91" s="2"/>
-      <c r="AO91" s="2"/>
-      <c r="AP91" s="2"/>
-      <c r="AQ91" s="2"/>
-      <c r="AR91" s="2"/>
-      <c r="AS91" s="2"/>
-      <c r="AT91" s="2"/>
-      <c r="AU91" s="2"/>
-      <c r="AV91" s="2"/>
-      <c r="AW91" s="2"/>
-      <c r="AX91" s="2"/>
-      <c r="AY91" s="2"/>
-      <c r="AZ91" s="2"/>
-      <c r="BA91" s="2"/>
-      <c r="BB91" s="2"/>
-      <c r="BC91" s="2"/>
-      <c r="BD91" s="2"/>
-      <c r="BE91" s="2"/>
-      <c r="BF91" s="2"/>
-      <c r="BG91" s="2"/>
-      <c r="BH91" s="2"/>
-      <c r="BI91" s="2"/>
-      <c r="BJ91" s="2"/>
-      <c r="BK91" s="2"/>
-      <c r="BL91" s="2"/>
-      <c r="BM91" s="2"/>
-      <c r="BN91" s="2"/>
-      <c r="BO91" s="2"/>
-      <c r="BP91" s="2"/>
-      <c r="BQ91" s="2"/>
-      <c r="BR91" s="2"/>
-      <c r="BS91" s="2"/>
-      <c r="BT91" s="2"/>
-      <c r="BU91" s="2"/>
-      <c r="BV91" s="2"/>
-      <c r="BW91" s="2"/>
-      <c r="BX91" s="2"/>
-      <c r="BY91" s="2"/>
-      <c r="BZ91" s="2"/>
-      <c r="CA91" s="2"/>
-    </row>
-    <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
-      <c r="M92" s="2"/>
-      <c r="N92" s="2"/>
-      <c r="O92" s="2"/>
-      <c r="P92" s="2"/>
-      <c r="Q92" s="2"/>
-      <c r="R92" s="2"/>
-      <c r="S92" s="2"/>
-      <c r="T92" s="2"/>
-      <c r="U92" s="2"/>
-      <c r="V92" s="2"/>
-      <c r="W92" s="2"/>
-      <c r="X92" s="2"/>
-      <c r="Y92" s="2"/>
-      <c r="Z92" s="2"/>
-      <c r="AA92" s="2"/>
-      <c r="AB92" s="2"/>
-      <c r="AC92" s="2"/>
-      <c r="AD92" s="2"/>
-      <c r="AE92" s="2"/>
-      <c r="AF92" s="2"/>
-      <c r="AG92" s="2"/>
-      <c r="AH92" s="2"/>
-      <c r="AI92" s="2"/>
-      <c r="AJ92" s="2"/>
-      <c r="AK92" s="2"/>
-      <c r="AL92" s="2"/>
-      <c r="AM92" s="2"/>
-      <c r="AN92" s="2"/>
-      <c r="AO92" s="2"/>
-      <c r="AP92" s="2"/>
-      <c r="AQ92" s="2"/>
-      <c r="AR92" s="2"/>
-      <c r="AS92" s="2"/>
-      <c r="AT92" s="2"/>
-      <c r="AU92" s="2"/>
-      <c r="AV92" s="2"/>
-      <c r="AW92" s="2"/>
-      <c r="AX92" s="2"/>
-      <c r="AY92" s="2"/>
-      <c r="AZ92" s="2"/>
-      <c r="BA92" s="2"/>
-      <c r="BB92" s="2"/>
-      <c r="BC92" s="2"/>
-      <c r="BD92" s="2"/>
-      <c r="BE92" s="2"/>
-      <c r="BF92" s="2"/>
-      <c r="BG92" s="2"/>
-      <c r="BH92" s="2"/>
-      <c r="BI92" s="2"/>
-      <c r="BJ92" s="2"/>
-      <c r="BK92" s="2"/>
-      <c r="BL92" s="2"/>
-      <c r="BM92" s="2"/>
-      <c r="BN92" s="2"/>
-      <c r="BO92" s="2"/>
-      <c r="BP92" s="2"/>
-      <c r="BQ92" s="2"/>
-      <c r="BR92" s="2"/>
-      <c r="BS92" s="2"/>
-      <c r="BT92" s="2"/>
-      <c r="BU92" s="2"/>
-      <c r="BV92" s="2"/>
-      <c r="BW92" s="2"/>
-      <c r="BX92" s="2"/>
-      <c r="BY92" s="2"/>
-      <c r="BZ92" s="2"/>
-      <c r="CA92" s="2"/>
-    </row>
-    <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
-      <c r="N93" s="2"/>
-      <c r="O93" s="2"/>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="2"/>
-      <c r="R93" s="2"/>
-      <c r="S93" s="2"/>
-      <c r="T93" s="2"/>
-      <c r="U93" s="2"/>
-      <c r="V93" s="2"/>
-      <c r="W93" s="2"/>
-      <c r="X93" s="2"/>
-      <c r="Y93" s="2"/>
-      <c r="Z93" s="2"/>
-      <c r="AA93" s="2"/>
-      <c r="AB93" s="2"/>
-      <c r="AC93" s="2"/>
-      <c r="AD93" s="2"/>
-      <c r="AE93" s="2"/>
-      <c r="AF93" s="2"/>
-      <c r="AG93" s="2"/>
-      <c r="AH93" s="2"/>
-      <c r="AI93" s="2"/>
-      <c r="AJ93" s="2"/>
-      <c r="AK93" s="2"/>
-      <c r="AL93" s="2"/>
-      <c r="AM93" s="2"/>
-      <c r="AN93" s="2"/>
-      <c r="AO93" s="2"/>
-      <c r="AP93" s="2"/>
-      <c r="AQ93" s="2"/>
-      <c r="AR93" s="2"/>
-      <c r="AS93" s="2"/>
-      <c r="AT93" s="2"/>
-      <c r="AU93" s="2"/>
-      <c r="AV93" s="2"/>
-      <c r="AW93" s="2"/>
-      <c r="AX93" s="2"/>
-      <c r="AY93" s="2"/>
-      <c r="AZ93" s="2"/>
-      <c r="BA93" s="2"/>
-      <c r="BB93" s="2"/>
-      <c r="BC93" s="2"/>
-      <c r="BD93" s="2"/>
-      <c r="BE93" s="2"/>
-      <c r="BF93" s="2"/>
-      <c r="BG93" s="2"/>
-      <c r="BH93" s="2"/>
-      <c r="BI93" s="2"/>
-      <c r="BJ93" s="2"/>
-      <c r="BK93" s="2"/>
-      <c r="BL93" s="2"/>
-      <c r="BM93" s="2"/>
-      <c r="BN93" s="2"/>
-      <c r="BO93" s="2"/>
-      <c r="BP93" s="2"/>
-      <c r="BQ93" s="2"/>
-      <c r="BR93" s="2"/>
-      <c r="BS93" s="2"/>
-      <c r="BT93" s="2"/>
-      <c r="BU93" s="2"/>
-      <c r="BV93" s="2"/>
-      <c r="BW93" s="2"/>
-      <c r="BX93" s="2"/>
-      <c r="BY93" s="2"/>
-      <c r="BZ93" s="2"/>
-      <c r="CA93" s="2"/>
+    <row r="91" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH91" s="0"/>
+      <c r="AMI91" s="0"/>
+      <c r="AMJ91" s="0"/>
+    </row>
+    <row r="92" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH92" s="0"/>
+      <c r="AMI92" s="0"/>
+      <c r="AMJ92" s="0"/>
+    </row>
+    <row r="93" s="2" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH93" s="0"/>
+      <c r="AMI93" s="0"/>
+      <c r="AMJ93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F94" s="2"/>
@@ -27956,6 +28144,240 @@
       <c r="BZ402" s="2"/>
       <c r="CA402" s="2"/>
     </row>
+    <row r="403" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F403" s="2"/>
+      <c r="G403" s="2"/>
+      <c r="H403" s="2"/>
+      <c r="I403" s="2"/>
+      <c r="J403" s="2"/>
+      <c r="K403" s="2"/>
+      <c r="L403" s="2"/>
+      <c r="M403" s="2"/>
+      <c r="N403" s="2"/>
+      <c r="O403" s="2"/>
+      <c r="P403" s="2"/>
+      <c r="Q403" s="2"/>
+      <c r="R403" s="2"/>
+      <c r="S403" s="2"/>
+      <c r="T403" s="2"/>
+      <c r="U403" s="2"/>
+      <c r="V403" s="2"/>
+      <c r="W403" s="2"/>
+      <c r="X403" s="2"/>
+      <c r="Y403" s="2"/>
+      <c r="Z403" s="2"/>
+      <c r="AA403" s="2"/>
+      <c r="AB403" s="2"/>
+      <c r="AC403" s="2"/>
+      <c r="AD403" s="2"/>
+      <c r="AE403" s="2"/>
+      <c r="AF403" s="2"/>
+      <c r="AG403" s="2"/>
+      <c r="AH403" s="2"/>
+      <c r="AI403" s="2"/>
+      <c r="AJ403" s="2"/>
+      <c r="AK403" s="2"/>
+      <c r="AL403" s="2"/>
+      <c r="AM403" s="2"/>
+      <c r="AN403" s="2"/>
+      <c r="AO403" s="2"/>
+      <c r="AP403" s="2"/>
+      <c r="AQ403" s="2"/>
+      <c r="AR403" s="2"/>
+      <c r="AS403" s="2"/>
+      <c r="AT403" s="2"/>
+      <c r="AU403" s="2"/>
+      <c r="AV403" s="2"/>
+      <c r="AW403" s="2"/>
+      <c r="AX403" s="2"/>
+      <c r="AY403" s="2"/>
+      <c r="AZ403" s="2"/>
+      <c r="BA403" s="2"/>
+      <c r="BB403" s="2"/>
+      <c r="BC403" s="2"/>
+      <c r="BD403" s="2"/>
+      <c r="BE403" s="2"/>
+      <c r="BF403" s="2"/>
+      <c r="BG403" s="2"/>
+      <c r="BH403" s="2"/>
+      <c r="BI403" s="2"/>
+      <c r="BJ403" s="2"/>
+      <c r="BK403" s="2"/>
+      <c r="BL403" s="2"/>
+      <c r="BM403" s="2"/>
+      <c r="BN403" s="2"/>
+      <c r="BO403" s="2"/>
+      <c r="BP403" s="2"/>
+      <c r="BQ403" s="2"/>
+      <c r="BR403" s="2"/>
+      <c r="BS403" s="2"/>
+      <c r="BT403" s="2"/>
+      <c r="BU403" s="2"/>
+      <c r="BV403" s="2"/>
+      <c r="BW403" s="2"/>
+      <c r="BX403" s="2"/>
+      <c r="BY403" s="2"/>
+      <c r="BZ403" s="2"/>
+      <c r="CA403" s="2"/>
+    </row>
+    <row r="404" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F404" s="2"/>
+      <c r="G404" s="2"/>
+      <c r="H404" s="2"/>
+      <c r="I404" s="2"/>
+      <c r="J404" s="2"/>
+      <c r="K404" s="2"/>
+      <c r="L404" s="2"/>
+      <c r="M404" s="2"/>
+      <c r="N404" s="2"/>
+      <c r="O404" s="2"/>
+      <c r="P404" s="2"/>
+      <c r="Q404" s="2"/>
+      <c r="R404" s="2"/>
+      <c r="S404" s="2"/>
+      <c r="T404" s="2"/>
+      <c r="U404" s="2"/>
+      <c r="V404" s="2"/>
+      <c r="W404" s="2"/>
+      <c r="X404" s="2"/>
+      <c r="Y404" s="2"/>
+      <c r="Z404" s="2"/>
+      <c r="AA404" s="2"/>
+      <c r="AB404" s="2"/>
+      <c r="AC404" s="2"/>
+      <c r="AD404" s="2"/>
+      <c r="AE404" s="2"/>
+      <c r="AF404" s="2"/>
+      <c r="AG404" s="2"/>
+      <c r="AH404" s="2"/>
+      <c r="AI404" s="2"/>
+      <c r="AJ404" s="2"/>
+      <c r="AK404" s="2"/>
+      <c r="AL404" s="2"/>
+      <c r="AM404" s="2"/>
+      <c r="AN404" s="2"/>
+      <c r="AO404" s="2"/>
+      <c r="AP404" s="2"/>
+      <c r="AQ404" s="2"/>
+      <c r="AR404" s="2"/>
+      <c r="AS404" s="2"/>
+      <c r="AT404" s="2"/>
+      <c r="AU404" s="2"/>
+      <c r="AV404" s="2"/>
+      <c r="AW404" s="2"/>
+      <c r="AX404" s="2"/>
+      <c r="AY404" s="2"/>
+      <c r="AZ404" s="2"/>
+      <c r="BA404" s="2"/>
+      <c r="BB404" s="2"/>
+      <c r="BC404" s="2"/>
+      <c r="BD404" s="2"/>
+      <c r="BE404" s="2"/>
+      <c r="BF404" s="2"/>
+      <c r="BG404" s="2"/>
+      <c r="BH404" s="2"/>
+      <c r="BI404" s="2"/>
+      <c r="BJ404" s="2"/>
+      <c r="BK404" s="2"/>
+      <c r="BL404" s="2"/>
+      <c r="BM404" s="2"/>
+      <c r="BN404" s="2"/>
+      <c r="BO404" s="2"/>
+      <c r="BP404" s="2"/>
+      <c r="BQ404" s="2"/>
+      <c r="BR404" s="2"/>
+      <c r="BS404" s="2"/>
+      <c r="BT404" s="2"/>
+      <c r="BU404" s="2"/>
+      <c r="BV404" s="2"/>
+      <c r="BW404" s="2"/>
+      <c r="BX404" s="2"/>
+      <c r="BY404" s="2"/>
+      <c r="BZ404" s="2"/>
+      <c r="CA404" s="2"/>
+    </row>
+    <row r="405" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F405" s="2"/>
+      <c r="G405" s="2"/>
+      <c r="H405" s="2"/>
+      <c r="I405" s="2"/>
+      <c r="J405" s="2"/>
+      <c r="K405" s="2"/>
+      <c r="L405" s="2"/>
+      <c r="M405" s="2"/>
+      <c r="N405" s="2"/>
+      <c r="O405" s="2"/>
+      <c r="P405" s="2"/>
+      <c r="Q405" s="2"/>
+      <c r="R405" s="2"/>
+      <c r="S405" s="2"/>
+      <c r="T405" s="2"/>
+      <c r="U405" s="2"/>
+      <c r="V405" s="2"/>
+      <c r="W405" s="2"/>
+      <c r="X405" s="2"/>
+      <c r="Y405" s="2"/>
+      <c r="Z405" s="2"/>
+      <c r="AA405" s="2"/>
+      <c r="AB405" s="2"/>
+      <c r="AC405" s="2"/>
+      <c r="AD405" s="2"/>
+      <c r="AE405" s="2"/>
+      <c r="AF405" s="2"/>
+      <c r="AG405" s="2"/>
+      <c r="AH405" s="2"/>
+      <c r="AI405" s="2"/>
+      <c r="AJ405" s="2"/>
+      <c r="AK405" s="2"/>
+      <c r="AL405" s="2"/>
+      <c r="AM405" s="2"/>
+      <c r="AN405" s="2"/>
+      <c r="AO405" s="2"/>
+      <c r="AP405" s="2"/>
+      <c r="AQ405" s="2"/>
+      <c r="AR405" s="2"/>
+      <c r="AS405" s="2"/>
+      <c r="AT405" s="2"/>
+      <c r="AU405" s="2"/>
+      <c r="AV405" s="2"/>
+      <c r="AW405" s="2"/>
+      <c r="AX405" s="2"/>
+      <c r="AY405" s="2"/>
+      <c r="AZ405" s="2"/>
+      <c r="BA405" s="2"/>
+      <c r="BB405" s="2"/>
+      <c r="BC405" s="2"/>
+      <c r="BD405" s="2"/>
+      <c r="BE405" s="2"/>
+      <c r="BF405" s="2"/>
+      <c r="BG405" s="2"/>
+      <c r="BH405" s="2"/>
+      <c r="BI405" s="2"/>
+      <c r="BJ405" s="2"/>
+      <c r="BK405" s="2"/>
+      <c r="BL405" s="2"/>
+      <c r="BM405" s="2"/>
+      <c r="BN405" s="2"/>
+      <c r="BO405" s="2"/>
+      <c r="BP405" s="2"/>
+      <c r="BQ405" s="2"/>
+      <c r="BR405" s="2"/>
+      <c r="BS405" s="2"/>
+      <c r="BT405" s="2"/>
+      <c r="BU405" s="2"/>
+      <c r="BV405" s="2"/>
+      <c r="BW405" s="2"/>
+      <c r="BX405" s="2"/>
+      <c r="BY405" s="2"/>
+      <c r="BZ405" s="2"/>
+      <c r="CA405" s="2"/>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="A1:E1"/>
@@ -27966,21 +28388,21 @@
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:E36"/>
     <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.590277777777778" header="0.511811023622047" footer="0"/>
@@ -27991,5 +28413,6 @@
 Santiago Ofreggia
 Gerente Comercial</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corregí el formato del precio
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -782,9 +782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9085320</xdr:colOff>
+      <xdr:colOff>9084960</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>427680</xdr:rowOff>
+      <xdr:rowOff>427320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -798,7 +798,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7351200" y="5624640"/>
-          <a:ext cx="4206240" cy="2905560"/>
+          <a:ext cx="4205880" cy="2905200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -821,10 +821,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.8"/>
@@ -1671,7 +1671,9 @@
       <c r="C11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="16" t="n">
+        <v>1212</v>
+      </c>
       <c r="E11" s="17" t="n">
         <f aca="false">B11*D11</f>
         <v>0</v>

</xml_diff>

<commit_message>
No se esta cambiando, intento pushear devuelta
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -23,15 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">JDN COMPANY RIEGO</t>
   </si>
   <si>
     <t xml:space="preserve">DIVISIÓN TABLE ESTACADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLIENTE</t>
   </si>
   <si>
     <t xml:space="preserve">Código</t>
@@ -106,13 +103,13 @@
     <t xml:space="preserve">PLAZO EJECUCIÓN OBRA</t>
   </si>
   <si>
-    <t xml:space="preserve">Plazo de ejecución de obra      10    días hábiles, de no existir problemas metereologicos.</t>
+    <t xml:space="preserve">Plazo de ejecución de obra 10  días hábiles, de no existir problemas metereologicos.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDEZ DE LA OFERTA</t>
   </si>
   <si>
-    <t xml:space="preserve">            días a partir de la fecha de la presente cotización.</t>
+    <t xml:space="preserve"> 5 días a partir de la fecha de la presente cotización.</t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
@@ -776,15 +773,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4879080</xdr:colOff>
+      <xdr:colOff>4816440</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9084960</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>427320</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -797,8 +794,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7351200" y="5624640"/>
-          <a:ext cx="4205880" cy="2905200"/>
+          <a:off x="7288560" y="5624640"/>
+          <a:ext cx="4268520" cy="2948400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -821,7 +818,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1081,9 +1078,7 @@
       <c r="CA3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1327,19 +1322,19 @@
     </row>
     <row r="7" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="E7" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1421,10 +1416,10 @@
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1586,7 +1581,7 @@
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="17"/>
@@ -1669,11 +1664,9 @@
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
-      <c r="D11" s="16" t="n">
-        <v>1212</v>
-      </c>
+      <c r="D11" s="16"/>
       <c r="E11" s="17" t="n">
         <f aca="false">B11*D11</f>
         <v>0</v>
@@ -1838,7 +1831,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="n">
@@ -2006,7 +1999,7 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="24" t="n">
         <f aca="false">SUM(E11:E14)</f>
@@ -2173,7 +2166,7 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="2"/>
@@ -2254,7 +2247,7 @@
     <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="32"/>
@@ -2341,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
@@ -2423,10 +2416,10 @@
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="36"/>
@@ -2508,10 +2501,10 @@
     <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="34"/>
       <c r="B21" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
@@ -2594,7 +2587,7 @@
       <c r="A22" s="34"/>
       <c r="B22" s="30"/>
       <c r="C22" s="34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
@@ -2676,10 +2669,10 @@
     <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="34"/>
       <c r="B23" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="36"/>
@@ -2761,10 +2754,10 @@
     <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="34"/>
       <c r="B24" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
@@ -2846,10 +2839,10 @@
     <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="34"/>
       <c r="B25" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
@@ -2932,7 +2925,7 @@
       <c r="A26" s="34"/>
       <c r="B26" s="30"/>
       <c r="C26" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="38"/>
@@ -3120,7 +3113,7 @@
     </row>
     <row r="28" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -3229,7 +3222,7 @@
     </row>
     <row r="29" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3338,7 +3331,7 @@
     </row>
     <row r="30" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
@@ -3447,7 +3440,7 @@
     </row>
     <row r="31" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
@@ -3556,7 +3549,7 @@
     </row>
     <row r="32" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
@@ -3772,7 +3765,7 @@
     </row>
     <row r="34" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -3881,7 +3874,7 @@
     </row>
     <row r="35" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
@@ -4152,7 +4145,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="49"/>
       <c r="C38" s="49"/>
@@ -4235,7 +4228,7 @@
     </row>
     <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>

</xml_diff>

<commit_message>
Intente borrar el lock y agrear un gitignore
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -779,9 +779,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2152440</xdr:colOff>
+      <xdr:colOff>2152080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>429480</xdr:rowOff>
+      <xdr:rowOff>429120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -795,7 +795,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12102480" y="5672880"/>
-          <a:ext cx="4139280" cy="2859120"/>
+          <a:ext cx="4138920" cy="2858760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -818,10 +818,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.8"/>

</xml_diff>

<commit_message>
Probando agregar solo texto
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -23,12 +23,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t xml:space="preserve">JDN COMPANY RIEGO</t>
   </si>
   <si>
     <t xml:space="preserve">DIVISIÓN TABLE ESTACADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">que esta</t>
   </si>
   <si>
     <t xml:space="preserve">Código</t>
@@ -110,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 5 días a partir de la fecha de la presente cotización.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
@@ -779,9 +785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2152080</xdr:colOff>
+      <xdr:colOff>2151720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>429120</xdr:rowOff>
+      <xdr:rowOff>428760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -795,7 +801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12102480" y="5672880"/>
-          <a:ext cx="4138920" cy="2858760"/>
+          <a:ext cx="4138560" cy="2858400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -818,10 +824,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.8"/>
@@ -1078,7 +1084,9 @@
       <c r="CA3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1322,19 +1330,19 @@
     </row>
     <row r="7" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1416,10 +1424,10 @@
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1581,7 +1589,7 @@
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="17"/>
@@ -1664,7 +1672,7 @@
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="17" t="n">
@@ -1831,7 +1839,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="n">
@@ -1999,7 +2007,7 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="24" t="n">
         <f aca="false">SUM(E11:E14)</f>
@@ -2166,7 +2174,7 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" s="29" t="n">
         <f aca="false">E14</f>
@@ -2250,7 +2258,7 @@
     <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="32"/>
@@ -2337,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
@@ -2419,10 +2427,10 @@
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="36"/>
@@ -2504,10 +2512,10 @@
     <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="34"/>
       <c r="B21" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
@@ -2590,7 +2598,7 @@
       <c r="A22" s="34"/>
       <c r="B22" s="30"/>
       <c r="C22" s="34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
@@ -2672,10 +2680,10 @@
     <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="34"/>
       <c r="B23" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="36"/>
@@ -2757,10 +2765,10 @@
     <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="34"/>
       <c r="B24" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
@@ -2842,10 +2850,10 @@
     <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="34"/>
       <c r="B25" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
@@ -2928,7 +2936,7 @@
       <c r="A26" s="34"/>
       <c r="B26" s="30"/>
       <c r="C26" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="38"/>
@@ -3116,7 +3124,7 @@
     </row>
     <row r="28" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -3225,7 +3233,7 @@
     </row>
     <row r="29" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3334,7 +3342,7 @@
     </row>
     <row r="30" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
@@ -3443,7 +3451,7 @@
     </row>
     <row r="31" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
@@ -3552,7 +3560,7 @@
     </row>
     <row r="32" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
@@ -3768,7 +3776,7 @@
     </row>
     <row r="34" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -3877,7 +3885,7 @@
     </row>
     <row r="35" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
@@ -3987,7 +3995,9 @@
     <row r="36" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="43"/>
       <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
+      <c r="C36" s="45" t="s">
+        <v>30</v>
+      </c>
       <c r="D36" s="46"/>
       <c r="E36" s="47"/>
       <c r="F36" s="2"/>
@@ -4148,7 +4158,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="49" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B38" s="49"/>
       <c r="C38" s="49"/>
@@ -4231,7 +4241,7 @@
     </row>
     <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>

</xml_diff>

<commit_message>
Hardcodee formatos desde appy y elimine imagen
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -23,15 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">JDN COMPANY RIEGO</t>
   </si>
   <si>
     <t xml:space="preserve">DIVISIÓN TABLE ESTACADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">que esta</t>
   </si>
   <si>
     <t xml:space="preserve">Código</t>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 5 días a partir de la fecha de la presente cotización.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES</t>
@@ -774,48 +768,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>537840</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2151720</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>428760</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12102480" y="5672880"/>
-          <a:ext cx="4138560" cy="2858400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -823,8 +775,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1084,9 +1036,7 @@
       <c r="CA3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1330,19 +1280,19 @@
     </row>
     <row r="7" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="E7" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1424,10 +1374,10 @@
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1589,7 +1539,7 @@
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="17"/>
@@ -1672,7 +1622,7 @@
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="17" t="n">
@@ -1839,7 +1789,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="n">
@@ -2007,10 +1957,10 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="24" t="n">
-        <f aca="false">SUM(E11:E14)</f>
+        <f aca="false">SUM(E11:E13)</f>
         <v>0</v>
       </c>
       <c r="F15" s="2"/>
@@ -2174,10 +2124,10 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="29" t="n">
-        <f aca="false">E14</f>
+        <f aca="false">E15</f>
         <v>0</v>
       </c>
       <c r="F17" s="2"/>
@@ -2258,7 +2208,7 @@
     <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="32"/>
@@ -2345,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
@@ -2427,10 +2377,10 @@
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="34"/>
       <c r="B20" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="36"/>
@@ -2512,10 +2462,10 @@
     <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="34"/>
       <c r="B21" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
@@ -2598,7 +2548,7 @@
       <c r="A22" s="34"/>
       <c r="B22" s="30"/>
       <c r="C22" s="34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
@@ -2680,10 +2630,10 @@
     <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="34"/>
       <c r="B23" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="36"/>
@@ -2765,10 +2715,10 @@
     <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="34"/>
       <c r="B24" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
@@ -2850,10 +2800,10 @@
     <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="34"/>
       <c r="B25" s="30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
@@ -2936,7 +2886,7 @@
       <c r="A26" s="34"/>
       <c r="B26" s="30"/>
       <c r="C26" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="38"/>
@@ -3124,7 +3074,7 @@
     </row>
     <row r="28" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -3233,7 +3183,7 @@
     </row>
     <row r="29" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3342,7 +3292,7 @@
     </row>
     <row r="30" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="41"/>
@@ -3451,7 +3401,7 @@
     </row>
     <row r="31" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
@@ -3560,7 +3510,7 @@
     </row>
     <row r="32" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="41"/>
@@ -3776,7 +3726,7 @@
     </row>
     <row r="34" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -3885,7 +3835,7 @@
     </row>
     <row r="35" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
@@ -3995,9 +3945,7 @@
     <row r="36" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="43"/>
       <c r="B36" s="44"/>
-      <c r="C36" s="45" t="s">
-        <v>30</v>
-      </c>
+      <c r="C36" s="45"/>
       <c r="D36" s="46"/>
       <c r="E36" s="47"/>
       <c r="F36" s="2"/>
@@ -4158,7 +4106,7 @@
     </row>
     <row r="38" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B38" s="49"/>
       <c r="C38" s="49"/>
@@ -4241,7 +4189,7 @@
     </row>
     <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39" s="50"/>
       <c r="C39" s="50"/>
@@ -28421,6 +28369,5 @@
 Santiago Ofreggia
 Gerente Comercial</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
saque total y anterior font
</commit_message>
<xml_diff>
--- a/plantillas/estacado.xlsx
+++ b/plantillas/estacado.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t xml:space="preserve">JDN COMPANY RIEGO</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Escalones</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Total $</t>
+    <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t xml:space="preserve">Medidas</t>
@@ -487,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,6 +564,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,9 +604,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="9" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -775,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1624,7 +1628,7 @@
       <c r="C11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="17" t="n">
         <f aca="false">B11*D11</f>
         <v>0</v>
@@ -1791,7 +1795,7 @@
       <c r="C13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="17" t="n">
         <f aca="false">D13*B13</f>
         <v>0</v>
@@ -1872,9 +1876,9 @@
       <c r="CA13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17"/>
       <c r="F14" s="2"/>
@@ -1953,13 +1957,13 @@
       <c r="CA14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="24" t="n">
+      <c r="E15" s="25" t="n">
         <f aca="false">SUM(E11:E13)</f>
         <v>0</v>
       </c>
@@ -2039,11 +2043,11 @@
       <c r="CA15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="26"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2120,16 +2124,11 @@
       <c r="CA16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="29" t="n">
-        <f aca="false">E15</f>
-        <v>0</v>
-      </c>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -2206,13 +2205,13 @@
       <c r="CA17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2289,16 +2288,16 @@
       <c r="CA18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34"/>
-      <c r="B19" s="30" t="n">
+      <c r="A19" s="35"/>
+      <c r="B19" s="31" t="n">
         <f aca="false">B11</f>
         <v>0</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2375,15 +2374,15 @@
       <c r="CA19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="30" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2460,15 +2459,15 @@
       <c r="CA20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="30" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2545,13 +2544,13 @@
       <c r="CA21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="34" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2628,15 +2627,15 @@
       <c r="CA22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="30" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2713,15 +2712,15 @@
       <c r="CA23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2798,15 +2797,15 @@
       <c r="CA24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="34"/>
-      <c r="B25" s="30" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2883,13 +2882,13 @@
       <c r="CA25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="34"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="34" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2966,11 +2965,11 @@
       <c r="CA26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -3073,13 +3072,13 @@
       <c r="DA27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3182,13 +3181,13 @@
       <c r="DA28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -3291,13 +3290,13 @@
       <c r="DA29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -3400,13 +3399,13 @@
       <c r="DA30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -3509,13 +3508,13 @@
       <c r="DA31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3618,11 +3617,11 @@
       <c r="DA32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -3725,13 +3724,13 @@
       <c r="DA33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -3834,13 +3833,13 @@
       <c r="DA34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -3943,11 +3942,11 @@
       <c r="DA35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="48"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -4024,11 +4023,11 @@
       <c r="CA36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="48"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -4105,13 +4104,13 @@
       <c r="CA37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -4188,13 +4187,13 @@
       <c r="CA38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -4271,11 +4270,11 @@
       <c r="CA39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="51"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>

</xml_diff>